<commit_message>
some changes in the excel file
</commit_message>
<xml_diff>
--- a/OD matrix for students.xlsx
+++ b/OD matrix for students.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seppe/Documents/IP1b/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9C38D3-EA38-8741-A679-944EF4E2CDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F04D59-B0E2-4E4C-8364-87B0A7A6480C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OD" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Heist</t>
   </si>
@@ -85,12 +85,21 @@
   <si>
     <t xml:space="preserve">total passengers </t>
   </si>
+  <si>
+    <t>OD (known) assaginment 1a</t>
+  </si>
+  <si>
+    <t>arriving</t>
+  </si>
+  <si>
+    <t>through</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,8 +137,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +184,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -213,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -234,6 +255,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -973,6 +1004,13 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -1661,6 +1699,13 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -3280,8 +3325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3783,10 +3828,10 @@
         <v>6227</v>
       </c>
       <c r="D15" s="12">
-        <f t="shared" ref="D15:N15" si="2">SUM(D5:D14)</f>
+        <f t="shared" ref="D15:L15" si="2">SUM(D5:D14)</f>
         <v>36073</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="22">
         <f t="shared" si="2"/>
         <v>34937</v>
       </c>
@@ -3802,7 +3847,7 @@
         <f t="shared" si="2"/>
         <v>58732</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="23">
         <f t="shared" si="2"/>
         <v>77082</v>
       </c>
@@ -3827,7 +3872,7 @@
         <v>53331</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
         <v>15</v>
       </c>
@@ -3836,12 +3881,61 @@
         <v>396810</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" ht="19" x14ac:dyDescent="0.25">
+      <c r="B19" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="20">
+        <f>14474+7718+4890</f>
+        <v>27082</v>
+      </c>
+      <c r="D21">
+        <f>43423+23155</f>
+        <v>66578</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="21">
+        <f>3491+8422</f>
+        <v>11913</v>
+      </c>
+      <c r="D22">
+        <f>1745+4227</f>
+        <v>5972</v>
+      </c>
       <c r="E22" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B19:L19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>